<commit_message>
try patch and stride part 1
</commit_message>
<xml_diff>
--- a/Percobaan.xlsx
+++ b/Percobaan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aria Berlian\Documents\rbm_sr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B534341B-3D47-429D-999C-2F7CBF9BA604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2525C2-77F1-4B42-930D-49CEA87629FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <author>tc={DFF06DD3-5EFA-4907-9060-D1A2CFEB100E}</author>
   </authors>
   <commentList>
-    <comment ref="V7" authorId="0" shapeId="0" xr:uid="{DFF06DD3-5EFA-4907-9060-D1A2CFEB100E}">
+    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{DFF06DD3-5EFA-4907-9060-D1A2CFEB100E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="22">
   <si>
     <t>Training_image</t>
   </si>
@@ -119,16 +119,19 @@
   <si>
     <t>layers avg</t>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="#,##0.000"/>
-    <numFmt numFmtId="169" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,12 +154,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -169,7 +166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,12 +176,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -269,7 +260,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -283,43 +274,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -610,7 +592,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="V7" dT="2024-03-15T23:15:28.77" personId="{30B4AD63-1A05-4C32-B2FE-8AED357CC1E1}" id="{DFF06DD3-5EFA-4907-9060-D1A2CFEB100E}">
+  <threadedComment ref="U3" dT="2024-03-15T23:15:28.77" personId="{30B4AD63-1A05-4C32-B2FE-8AED357CC1E1}" id="{DFF06DD3-5EFA-4907-9060-D1A2CFEB100E}">
     <text>Notes:
 1. layers [24, 12, 48] best</text>
   </threadedComment>
@@ -619,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V45"/>
+  <dimension ref="A1:Y64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -649,7 +631,7 @@
     <col min="21" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -702,11 +684,14 @@
         <v>19</v>
       </c>
       <c r="T1" s="9"/>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -743,14 +728,15 @@
       <c r="T2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="1"/>
+      <c r="X2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -816,16 +802,16 @@
         <f>(N3+P3+R3)/3</f>
         <v>0.98292666666666673</v>
       </c>
-      <c r="U3" s="2">
+      <c r="X3" s="2">
         <f>(S3+S6+S9)/3</f>
         <v>30.584555555555553</v>
       </c>
-      <c r="V3" s="2">
+      <c r="Y3" s="2">
         <f>(T3+T6+T9)/3</f>
         <v>0.93487888888888893</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -846,7 +832,7 @@
         <v>15625</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G40" si="1">D4*D4*3</f>
+        <f t="shared" ref="G4:G12" si="1">D4*D4*3</f>
         <v>48</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -884,23 +870,23 @@
         <v>0.98543999999999998</v>
       </c>
       <c r="S4" s="7">
-        <f t="shared" ref="S4:S28" si="2">(M4+O4+Q4)/3</f>
+        <f t="shared" ref="S4:S12" si="2">(M4+O4+Q4)/3</f>
         <v>35.451666666666668</v>
       </c>
       <c r="T4" s="10">
-        <f t="shared" ref="T4:T26" si="3">(N4+P4+R4)/3</f>
+        <f t="shared" ref="T4:T12" si="3">(N4+P4+R4)/3</f>
         <v>0.98313000000000006</v>
       </c>
-      <c r="U4" s="2">
-        <f t="shared" ref="U4:U5" si="4">(S4+S7+S10)/3</f>
+      <c r="X4" s="2">
+        <f>(S4+S7+S10)/3</f>
         <v>30.611888888888888</v>
       </c>
-      <c r="V4" s="2">
-        <f t="shared" ref="V4:V5" si="5">(T4+T7+T10)/3</f>
+      <c r="Y4" s="2">
+        <f>(T4+T7+T10)/3</f>
         <v>0.93524888888888891</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -966,16 +952,16 @@
         <f t="shared" si="3"/>
         <v>0.98331333333333337</v>
       </c>
-      <c r="U5" s="2">
-        <f t="shared" si="4"/>
+      <c r="X5" s="2">
+        <f>(S5+S8+S11)/3</f>
         <v>30.716666666666665</v>
       </c>
-      <c r="V5" s="2">
-        <f t="shared" si="5"/>
+      <c r="Y5" s="2">
+        <f>(T5+T8+T11)/3</f>
         <v>0.93588555555555553</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1042,7 +1028,7 @@
         <v>0.95061666666666655</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1109,7 +1095,7 @@
         <v>0.95072666666666661</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1176,7 +1162,7 @@
         <v>0.95127000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1243,7 +1229,7 @@
         <v>0.87109333333333339</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1310,7 +1296,7 @@
         <v>0.87189000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1377,7 +1363,7 @@
         <v>0.87307333333333326</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1405,7 +1391,7 @@
         <v>13</v>
       </c>
       <c r="I12" s="2" t="str">
-        <f t="shared" ref="I12:I19" si="6">"[" &amp;G12/2&amp; "," &amp;G12/4&amp;  "," &amp;G12&amp;"]"</f>
+        <f t="shared" ref="I12:I27" si="4">"[" &amp;G12/2&amp; "," &amp;G12/4&amp;  "," &amp;G12&amp;"]"</f>
         <v>[1,5,0,75,3]</v>
       </c>
       <c r="J12" s="2">
@@ -1416,215 +1402,263 @@
       </c>
       <c r="L12" s="2">
         <v>1</v>
+      </c>
+      <c r="M12" s="7">
+        <v>13.4</v>
+      </c>
+      <c r="N12" s="13">
+        <v>0.70745999999999998</v>
+      </c>
+      <c r="O12" s="7">
+        <v>13.291</v>
+      </c>
+      <c r="P12" s="10">
+        <v>0.63529000000000002</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>12.954000000000001</v>
+      </c>
+      <c r="R12" s="10">
+        <v>0.73517999999999994</v>
       </c>
       <c r="S12" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13.215000000000002</v>
       </c>
       <c r="T12" s="10">
         <f t="shared" si="3"/>
+        <v>0.69264333333333339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>128</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <f>((B13-D13)/E13 + 1)^2</f>
+        <v>16129</v>
+      </c>
+      <c r="G13" s="2">
+        <f>D13*D13*3</f>
+        <v>12</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[6,3,12]</v>
+      </c>
+      <c r="J13" s="2">
+        <v>50</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="7">
+        <v>30.204000000000001</v>
+      </c>
+      <c r="N13" s="13">
+        <v>0.97638999999999998</v>
+      </c>
+      <c r="O13" s="7">
+        <v>36.664999999999999</v>
+      </c>
+      <c r="P13" s="10">
+        <v>0.97962000000000005</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>35.277000000000001</v>
+      </c>
+      <c r="R13" s="10">
+        <v>0.98126999999999998</v>
+      </c>
+      <c r="S13" s="7">
+        <f>(M13+O13+Q13)/3</f>
+        <v>34.048666666666669</v>
+      </c>
+      <c r="T13" s="10">
+        <f>(N13+P13+R13)/3</f>
+        <v>0.97909333333333326</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>128</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <f>((B14-D14)/E14 + 1)^2</f>
+        <v>15876</v>
+      </c>
+      <c r="G14" s="2">
+        <f>D14*D14*3</f>
+        <v>27</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[13,5,6,75,27]</v>
+      </c>
+      <c r="J14" s="2">
+        <v>50</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="M14" s="7">
+        <v>31.423999999999999</v>
+      </c>
+      <c r="N14" s="13">
+        <v>0.98114999999999997</v>
+      </c>
+      <c r="O14" s="7">
+        <v>38.476999999999997</v>
+      </c>
+      <c r="P14" s="10">
+        <v>0.98340000000000005</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>37.115000000000002</v>
+      </c>
+      <c r="R14" s="10">
+        <v>0.98529</v>
+      </c>
+      <c r="S14" s="7">
+        <f t="shared" ref="S14:S27" si="5">(M14+O14+Q14)/3</f>
+        <v>35.671999999999997</v>
+      </c>
+      <c r="T14" s="10">
+        <f t="shared" ref="T14:T27" si="6">(N14+P14+R14)/3</f>
+        <v>0.98328000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2">
+        <v>128</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>4</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2</v>
+      </c>
+      <c r="F15" s="2">
+        <f>((B15-D15)/E15 + 1)^2</f>
+        <v>3969</v>
+      </c>
+      <c r="G15" s="2">
+        <f>D15*D15*3</f>
+        <v>48</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[24,12,48]</v>
+      </c>
+      <c r="J15" s="2">
+        <v>50</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="S15" s="7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="14">
-        <v>128</v>
-      </c>
-      <c r="C13" s="14">
-        <v>2</v>
-      </c>
-      <c r="D13" s="14">
-        <v>1</v>
-      </c>
-      <c r="E13" s="14">
-        <v>2</v>
-      </c>
-      <c r="F13" s="14">
-        <f t="shared" si="0"/>
-        <v>4160.25</v>
-      </c>
-      <c r="G13" s="14">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="14" t="str">
+      <c r="T15" s="10">
         <f t="shared" si="6"/>
-        <v>[1,5,0,75,3]</v>
-      </c>
-      <c r="J13" s="14">
-        <v>50</v>
-      </c>
-      <c r="K13" s="14">
-        <v>1</v>
-      </c>
-      <c r="L13" s="14">
-        <v>1</v>
-      </c>
-      <c r="M13" s="15"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="15">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T13" s="17">
-        <f t="shared" si="3"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2">
+        <v>128</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>4</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4</v>
+      </c>
+      <c r="F16" s="2">
+        <f>((B16-D16)/E16 + 1)^2</f>
+        <v>1024</v>
+      </c>
+      <c r="G16" s="2">
+        <f>D16*D16*3</f>
+        <v>48</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[24,12,48]</v>
+      </c>
+      <c r="J16" s="2">
+        <v>50</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
+      <c r="S16" s="7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2">
-        <v>128</v>
-      </c>
-      <c r="C14" s="2">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2">
-        <v>2</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2">
-        <f t="shared" si="0"/>
-        <v>16129</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="2" t="str">
+      <c r="T16" s="10">
         <f t="shared" si="6"/>
-        <v>[6,3,12]</v>
-      </c>
-      <c r="J14" s="2">
-        <v>50</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1</v>
-      </c>
-      <c r="L14" s="2">
-        <v>1</v>
-      </c>
-      <c r="S14" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T14" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2">
-        <v>128</v>
-      </c>
-      <c r="C15" s="2">
-        <v>2</v>
-      </c>
-      <c r="D15" s="2">
-        <v>2</v>
-      </c>
-      <c r="E15" s="2">
-        <v>2</v>
-      </c>
-      <c r="F15" s="2">
-        <f t="shared" si="0"/>
-        <v>4096</v>
-      </c>
-      <c r="G15" s="2">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>[6,3,12]</v>
-      </c>
-      <c r="J15" s="2">
-        <v>50</v>
-      </c>
-      <c r="K15" s="2">
-        <v>1</v>
-      </c>
-      <c r="L15" s="2">
-        <v>1</v>
-      </c>
-      <c r="S15" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T15" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="2">
-        <v>128</v>
-      </c>
-      <c r="C16" s="2">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2">
-        <v>6</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2">
-        <f t="shared" si="0"/>
-        <v>15129</v>
-      </c>
-      <c r="G16" s="2">
-        <f t="shared" si="1"/>
-        <v>108</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>[54,27,108]</v>
-      </c>
-      <c r="J16" s="2">
-        <v>50</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1</v>
-      </c>
-      <c r="L16" s="2">
-        <v>1</v>
-      </c>
-      <c r="S16" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T16" s="10">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1642,39 +1676,57 @@
         <v>6</v>
       </c>
       <c r="E17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="0"/>
-        <v>3844</v>
+        <f>((B17-D17)/E17 + 1)^2</f>
+        <v>15129</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="1"/>
+        <f>D17*D17*3</f>
         <v>108</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I17" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[54,27,108]</v>
+      </c>
+      <c r="J17" s="2">
+        <v>50</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1</v>
+      </c>
+      <c r="M17" s="7">
+        <v>30.745999999999999</v>
+      </c>
+      <c r="N17" s="13">
+        <v>0.98057000000000005</v>
+      </c>
+      <c r="O17" s="7">
+        <v>38.473999999999997</v>
+      </c>
+      <c r="P17" s="10">
+        <v>0.98407</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>37.427999999999997</v>
+      </c>
+      <c r="R17" s="10">
+        <v>0.98604999999999998</v>
+      </c>
+      <c r="S17" s="7">
+        <f t="shared" si="5"/>
+        <v>35.54933333333333</v>
+      </c>
+      <c r="T17" s="10">
         <f t="shared" si="6"/>
-        <v>[54,27,108]</v>
-      </c>
-      <c r="J17" s="2">
-        <v>50</v>
-      </c>
-      <c r="K17" s="2">
-        <v>1</v>
-      </c>
-      <c r="L17" s="2">
-        <v>1</v>
-      </c>
-      <c r="S17" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T17" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.98356333333333346</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
@@ -1688,33 +1740,60 @@
         <v>2</v>
       </c>
       <c r="D18" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="0"/>
-        <v>14641</v>
+        <f>((B18-D18)/E18 + 1)^2</f>
+        <v>3844</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="1"/>
-        <v>192</v>
+        <f>D18*D18*3</f>
+        <v>108</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I18" s="2" t="str">
-        <f>"[" &amp;G18/2&amp; "," &amp;G18/4&amp;  "," &amp;G18&amp;"]"</f>
-        <v>[96,48,192]</v>
+        <f t="shared" si="4"/>
+        <v>[54,27,108]</v>
+      </c>
+      <c r="J18" s="2">
+        <v>50</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="7">
+        <v>30.587</v>
+      </c>
+      <c r="N18" s="13">
+        <v>0.96343000000000001</v>
+      </c>
+      <c r="O18" s="7">
+        <v>36.994999999999997</v>
+      </c>
+      <c r="P18" s="10">
+        <v>0.96157999999999999</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>36.076000000000001</v>
+      </c>
+      <c r="R18" s="10">
+        <v>0.94810000000000005</v>
       </c>
       <c r="S18" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>34.55266666666666</v>
       </c>
       <c r="T18" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>0.95770333333333335</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
@@ -1728,32 +1807,41 @@
         <v>2</v>
       </c>
       <c r="D19" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E19" s="2">
         <v>2</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="0"/>
-        <v>3721</v>
+        <f>((B19-D19)/E19 + 1)^2</f>
+        <v>4096</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="1"/>
-        <v>192</v>
+        <f>D19*D19*3</f>
+        <v>12</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I19" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[6,3,12]</v>
+      </c>
+      <c r="J19" s="2">
+        <v>50</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+      <c r="S19" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T19" s="10">
         <f t="shared" si="6"/>
-        <v>[96,48,192]</v>
-      </c>
-      <c r="S19" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T19" s="10">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1761,23 +1849,48 @@
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B20" s="2">
+        <v>128</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <f>((B20-D20)/E20 + 1)^2</f>
+        <v>14641</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="1"/>
+        <f>D20*D20*3</f>
+        <v>192</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[96,48,192]</v>
+      </c>
+      <c r="J20" s="2">
+        <v>50</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
+      <c r="S20" s="7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S20" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="T20" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1785,23 +1898,48 @@
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B21" s="2">
+        <v>128</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2">
+        <f>((B21-D21)/E21 + 1)^2</f>
+        <v>3721</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="1"/>
+        <f>D21*D21*3</f>
+        <v>192</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[96,48,192]</v>
+      </c>
+      <c r="J21" s="2">
+        <v>50</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
+      <c r="S21" s="7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S21" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="T21" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1809,23 +1947,48 @@
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B22" s="2">
+        <v>128</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+      <c r="F22" s="2">
+        <f>((B22-D22)/E22 + 1)^2</f>
+        <v>1681</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="1"/>
+        <f>D22*D22*3</f>
+        <v>192</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[96,48,192]</v>
+      </c>
+      <c r="J22" s="2">
+        <v>50</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
+      <c r="S22" s="7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S22" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="T22" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1833,20 +1996,48 @@
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B23" s="2">
+        <v>128</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2">
+        <v>4</v>
+      </c>
+      <c r="F23" s="2">
+        <f>((B23-D23)/E23 + 1)^2</f>
+        <v>961</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="1"/>
+        <f>D23*D23*3</f>
+        <v>192</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[96,48,192]</v>
+      </c>
+      <c r="J23" s="2">
+        <v>50</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+      <c r="S23" s="7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S23" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="T23" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1854,239 +2045,228 @@
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B24" s="2">
+        <v>128</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>8</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2">
+        <f>((B24-D24)/E24 + 1)^2</f>
+        <v>625</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="1"/>
+        <f>D24*D24*3</f>
+        <v>192</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[96,48,192]</v>
+      </c>
+      <c r="J24" s="2">
+        <v>50</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1</v>
+      </c>
+      <c r="S24" s="7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S24" s="7">
-        <f t="shared" si="2"/>
+      <c r="T24" s="10">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T24" s="10">
-        <f t="shared" si="3"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="2">
+        <v>128</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2">
+        <v>6</v>
+      </c>
+      <c r="F25" s="2">
+        <f>((B25-D25)/E25 + 1)^2</f>
+        <v>441</v>
+      </c>
+      <c r="G25" s="2">
+        <f>D25*D25*3</f>
+        <v>192</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[96,48,192]</v>
+      </c>
+      <c r="J25" s="2">
+        <v>50</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1</v>
+      </c>
+      <c r="S25" s="7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F25" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="1"/>
+      <c r="T25" s="10">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="S25" s="7">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="2">
+        <v>128</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2">
+        <v>8</v>
+      </c>
+      <c r="E26" s="2">
+        <v>8</v>
+      </c>
+      <c r="F26" s="2">
+        <f>((B26-D26)/E26 + 1)^2</f>
+        <v>256</v>
+      </c>
+      <c r="G26" s="2">
+        <f>D26*D26*3</f>
+        <v>192</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[96,48,192]</v>
+      </c>
+      <c r="J26" s="2">
+        <v>50</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1</v>
+      </c>
+      <c r="L26" s="2">
+        <v>1</v>
+      </c>
+      <c r="S26" s="7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="T25" s="10">
-        <f t="shared" si="3"/>
+      <c r="T26" s="10">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F26" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G26" s="2">
-        <f t="shared" si="1"/>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2048</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2">
+        <v>32</v>
+      </c>
+      <c r="E27" s="2">
+        <v>16</v>
+      </c>
+      <c r="F27" s="2">
+        <f>((B27-D27)/E27 + 1)^2</f>
+        <v>16129</v>
+      </c>
+      <c r="G27" s="2">
+        <f>D27*D27*3</f>
+        <v>3072</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>[1536,768,3072]</v>
+      </c>
+      <c r="J27" s="2">
+        <v>50</v>
+      </c>
+      <c r="K27" s="2">
+        <v>1</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1</v>
+      </c>
+      <c r="S27" s="7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S26" s="7">
-        <f t="shared" si="2"/>
+      <c r="T27" s="10">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T26" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F27" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G27" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S27" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F28" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G28" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S28" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="A28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="2">
+        <v>128</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F29" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G29" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F30" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G30" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F31" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G31" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F32" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G32" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F33" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F34" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G34" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F35" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G35" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F36" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G36" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F37" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G37" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F38" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G38" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F39" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G39" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F40" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G40" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F41" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="42" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F42" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="43" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F43" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="44" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F44" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="45" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F45" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="A29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="2">
+        <v>128</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J47" s="14"/>
+    </row>
+    <row r="64" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J64" s="14"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
experiment on small image
</commit_message>
<xml_diff>
--- a/Percobaan.xlsx
+++ b/Percobaan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aria Berlian\Documents\rbm_sr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2525C2-77F1-4B42-930D-49CEA87629FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA754093-1090-4BF4-8238-ED8D792C0CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,10 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Notes:
-1. layers [24, 12, 48] best</t>
+1. layers [24, 12, 48] best
+Reply:
+    2. size: patch:stride = 128:3:1 best
+Alt1 = 128:6:1; Alt2 = 128:8:1</t>
       </text>
     </comment>
   </commentList>
@@ -55,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="21">
   <si>
     <t>Training_image</t>
   </si>
@@ -115,9 +118,6 @@
   </si>
   <si>
     <t>Average</t>
-  </si>
-  <si>
-    <t>layers avg</t>
   </si>
   <si>
     <t>Notes</t>
@@ -301,7 +301,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -596,15 +596,19 @@
     <text>Notes:
 1. layers [24, 12, 48] best</text>
   </threadedComment>
+  <threadedComment ref="U3" dT="2024-03-17T03:42:29.83" personId="{30B4AD63-1A05-4C32-B2FE-8AED357CC1E1}" id="{83EEB583-2614-4465-B0EB-3B308A380AC0}" parentId="{DFF06DD3-5EFA-4907-9060-D1A2CFEB100E}">
+    <text>2. size: patch:stride = 128:3:1 best
+Alt1 = 128:6:1; Alt2 = 128:8:1</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y64"/>
+  <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -631,7 +635,7 @@
     <col min="21" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -685,13 +689,10 @@
       </c>
       <c r="T1" s="9"/>
       <c r="U1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -729,14 +730,8 @@
         <v>10</v>
       </c>
       <c r="U2" s="1"/>
-      <c r="X2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -753,7 +748,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F45" si="0">((B3-D3)/E3 + 1)^2</f>
+        <f>((B3-D3)/E3 + 1)^2</f>
         <v>15625</v>
       </c>
       <c r="G3" s="2">
@@ -802,16 +797,8 @@
         <f>(N3+P3+R3)/3</f>
         <v>0.98292666666666673</v>
       </c>
-      <c r="X3" s="2">
-        <f>(S3+S6+S9)/3</f>
-        <v>30.584555555555553</v>
-      </c>
-      <c r="Y3" s="2">
-        <f>(T3+T6+T9)/3</f>
-        <v>0.93487888888888893</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -828,11 +815,11 @@
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="0"/>
+        <f>((B4-D4)/E4 + 1)^2</f>
         <v>15625</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G12" si="1">D4*D4*3</f>
+        <f>D4*D4*3</f>
         <v>48</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -870,23 +857,15 @@
         <v>0.98543999999999998</v>
       </c>
       <c r="S4" s="7">
-        <f t="shared" ref="S4:S12" si="2">(M4+O4+Q4)/3</f>
+        <f>(M4+O4+Q4)/3</f>
         <v>35.451666666666668</v>
       </c>
       <c r="T4" s="10">
-        <f t="shared" ref="T4:T12" si="3">(N4+P4+R4)/3</f>
+        <f>(N4+P4+R4)/3</f>
         <v>0.98313000000000006</v>
       </c>
-      <c r="X4" s="2">
-        <f>(S4+S7+S10)/3</f>
-        <v>30.611888888888888</v>
-      </c>
-      <c r="Y4" s="2">
-        <f>(T4+T7+T10)/3</f>
-        <v>0.93524888888888891</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -903,11 +882,11 @@
         <v>1</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="0"/>
+        <f>((B5-D5)/E5 + 1)^2</f>
         <v>15625</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="1"/>
+        <f>D5*D5*3</f>
         <v>48</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -945,23 +924,15 @@
         <v>0.98585</v>
       </c>
       <c r="S5" s="7">
-        <f t="shared" si="2"/>
+        <f>(M5+O5+Q5)/3</f>
         <v>35.490333333333332</v>
       </c>
       <c r="T5" s="10">
-        <f t="shared" si="3"/>
+        <f>(N5+P5+R5)/3</f>
         <v>0.98331333333333337</v>
       </c>
-      <c r="X5" s="2">
-        <f>(S5+S8+S11)/3</f>
-        <v>30.716666666666665</v>
-      </c>
-      <c r="Y5" s="2">
-        <f>(T5+T8+T11)/3</f>
-        <v>0.93588555555555553</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -978,11 +949,11 @@
         <v>1</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="0"/>
+        <f>((B6-D6)/E6 + 1)^2</f>
         <v>15625</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="1"/>
+        <f>D6*D6*3</f>
         <v>48</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -1020,15 +991,15 @@
         <v>0.95911000000000002</v>
       </c>
       <c r="S6" s="7">
-        <f t="shared" si="2"/>
+        <f>(M6+O6+Q6)/3</f>
         <v>30.425000000000001</v>
       </c>
       <c r="T6" s="10">
-        <f t="shared" si="3"/>
+        <f>(N6+P6+R6)/3</f>
         <v>0.95061666666666655</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1045,11 +1016,11 @@
         <v>1</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="0"/>
+        <f>((B7-D7)/E7 + 1)^2</f>
         <v>15625</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="1"/>
+        <f>D7*D7*3</f>
         <v>48</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -1087,15 +1058,15 @@
         <v>0.95923000000000003</v>
       </c>
       <c r="S7" s="7">
-        <f t="shared" si="2"/>
+        <f>(M7+O7+Q7)/3</f>
         <v>30.416</v>
       </c>
       <c r="T7" s="10">
-        <f t="shared" si="3"/>
+        <f>(N7+P7+R7)/3</f>
         <v>0.95072666666666661</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1112,11 +1083,11 @@
         <v>1</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="0"/>
+        <f>((B8-D8)/E8 + 1)^2</f>
         <v>15625</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" si="1"/>
+        <f>D8*D8*3</f>
         <v>48</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -1154,15 +1125,15 @@
         <v>0.95950000000000002</v>
       </c>
       <c r="S8" s="7">
-        <f t="shared" si="2"/>
+        <f>(M8+O8+Q8)/3</f>
         <v>30.585333333333335</v>
       </c>
       <c r="T8" s="10">
-        <f t="shared" si="3"/>
+        <f>(N8+P8+R8)/3</f>
         <v>0.95127000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1179,11 +1150,11 @@
         <v>1</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="0"/>
+        <f>((B9-D9)/E9 + 1)^2</f>
         <v>15625</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="1"/>
+        <f>D9*D9*3</f>
         <v>48</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -1221,15 +1192,15 @@
         <v>0.89280999999999999</v>
       </c>
       <c r="S9" s="7">
-        <f t="shared" si="2"/>
+        <f>(M9+O9+Q9)/3</f>
         <v>25.913</v>
       </c>
       <c r="T9" s="10">
-        <f t="shared" si="3"/>
+        <f>(N9+P9+R9)/3</f>
         <v>0.87109333333333339</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1246,11 +1217,11 @@
         <v>1</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="0"/>
+        <f>((B10-D10)/E10 + 1)^2</f>
         <v>15625</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" si="1"/>
+        <f>D10*D10*3</f>
         <v>48</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -1288,15 +1259,15 @@
         <v>0.89370000000000005</v>
       </c>
       <c r="S10" s="7">
-        <f t="shared" si="2"/>
+        <f>(M10+O10+Q10)/3</f>
         <v>25.968</v>
       </c>
       <c r="T10" s="10">
-        <f t="shared" si="3"/>
+        <f>(N10+P10+R10)/3</f>
         <v>0.87189000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1313,11 +1284,11 @@
         <v>1</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="0"/>
+        <f>((B11-D11)/E11 + 1)^2</f>
         <v>15625</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="1"/>
+        <f>D11*D11*3</f>
         <v>48</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -1355,15 +1326,15 @@
         <v>0.89331000000000005</v>
       </c>
       <c r="S11" s="7">
-        <f t="shared" si="2"/>
+        <f>(M11+O11+Q11)/3</f>
         <v>26.074333333333332</v>
       </c>
       <c r="T11" s="10">
-        <f t="shared" si="3"/>
+        <f>(N11+P11+R11)/3</f>
         <v>0.87307333333333326</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1380,18 +1351,18 @@
         <v>1</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="0"/>
+        <f>((B12-D12)/E12 + 1)^2</f>
         <v>16384</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="1"/>
+        <f>D12*D12*3</f>
         <v>3</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I12" s="2" t="str">
-        <f t="shared" ref="I12:I27" si="4">"[" &amp;G12/2&amp; "," &amp;G12/4&amp;  "," &amp;G12&amp;"]"</f>
+        <f>"[" &amp;G12/2&amp; "," &amp;G12/4&amp;  "," &amp;G12&amp;"]"</f>
         <v>[1,5,0,75,3]</v>
       </c>
       <c r="J12" s="2">
@@ -1422,15 +1393,15 @@
         <v>0.73517999999999994</v>
       </c>
       <c r="S12" s="7">
-        <f t="shared" si="2"/>
+        <f>(M12+O12+Q12)/3</f>
         <v>13.215000000000002</v>
       </c>
       <c r="T12" s="10">
-        <f t="shared" si="3"/>
+        <f>(N12+P12+R12)/3</f>
         <v>0.69264333333333339</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1458,7 +1429,7 @@
         <v>13</v>
       </c>
       <c r="I13" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G13/2&amp; "," &amp;G13/4&amp;  "," &amp;G13&amp;"]"</f>
         <v>[6,3,12]</v>
       </c>
       <c r="J13" s="2">
@@ -1497,7 +1468,7 @@
         <v>0.97909333333333326</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1525,7 +1496,7 @@
         <v>13</v>
       </c>
       <c r="I14" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G14/2&amp; "," &amp;G14/4&amp;  "," &amp;G14&amp;"]"</f>
         <v>[13,5,6,75,27]</v>
       </c>
       <c r="J14" s="2">
@@ -1556,15 +1527,15 @@
         <v>0.98529</v>
       </c>
       <c r="S14" s="7">
-        <f t="shared" ref="S14:S27" si="5">(M14+O14+Q14)/3</f>
+        <f>(M14+O14+Q14)/3</f>
         <v>35.671999999999997</v>
       </c>
       <c r="T14" s="10">
-        <f t="shared" ref="T14:T27" si="6">(N14+P14+R14)/3</f>
+        <f>(N14+P14+R14)/3</f>
         <v>0.98328000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1592,7 +1563,7 @@
         <v>13</v>
       </c>
       <c r="I15" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G15/2&amp; "," &amp;G15/4&amp;  "," &amp;G15&amp;"]"</f>
         <v>[24,12,48]</v>
       </c>
       <c r="J15" s="2">
@@ -1604,16 +1575,34 @@
       <c r="L15" s="2">
         <v>1</v>
       </c>
+      <c r="M15" s="7">
+        <v>30.222999999999999</v>
+      </c>
+      <c r="N15" s="13">
+        <v>0.92786000000000002</v>
+      </c>
+      <c r="O15" s="7">
+        <v>33.256999999999998</v>
+      </c>
+      <c r="P15" s="10">
+        <v>0.88092999999999999</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>32.756999999999998</v>
+      </c>
+      <c r="R15" s="10">
+        <v>0.83133999999999997</v>
+      </c>
       <c r="S15" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>(M15+O15+Q15)/3</f>
+        <v>32.079000000000001</v>
       </c>
       <c r="T15" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+        <f>(N15+P15+R15)/3</f>
+        <v>0.8800433333333334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1641,7 +1630,7 @@
         <v>13</v>
       </c>
       <c r="I16" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G16/2&amp; "," &amp;G16/4&amp;  "," &amp;G16&amp;"]"</f>
         <v>[24,12,48]</v>
       </c>
       <c r="J16" s="2">
@@ -1653,13 +1642,31 @@
       <c r="L16" s="2">
         <v>1</v>
       </c>
+      <c r="M16" s="7">
+        <v>30.202999999999999</v>
+      </c>
+      <c r="N16" s="13">
+        <v>0.91878000000000004</v>
+      </c>
+      <c r="O16" s="7">
+        <v>36.994</v>
+      </c>
+      <c r="P16" s="10">
+        <v>0.95967000000000002</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>34.5</v>
+      </c>
+      <c r="R16" s="10">
+        <v>0.89132999999999996</v>
+      </c>
       <c r="S16" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>(M16+O16+Q16)/3</f>
+        <v>33.899000000000001</v>
       </c>
       <c r="T16" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>(N16+P16+R16)/3</f>
+        <v>0.92325999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.35">
@@ -1690,7 +1697,7 @@
         <v>13</v>
       </c>
       <c r="I17" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G17/2&amp; "," &amp;G17/4&amp;  "," &amp;G17&amp;"]"</f>
         <v>[54,27,108]</v>
       </c>
       <c r="J17" s="2">
@@ -1721,11 +1728,11 @@
         <v>0.98604999999999998</v>
       </c>
       <c r="S17" s="7">
-        <f t="shared" si="5"/>
+        <f>(M17+O17+Q17)/3</f>
         <v>35.54933333333333</v>
       </c>
       <c r="T17" s="10">
-        <f t="shared" si="6"/>
+        <f>(N17+P17+R17)/3</f>
         <v>0.98356333333333346</v>
       </c>
     </row>
@@ -1757,7 +1764,7 @@
         <v>13</v>
       </c>
       <c r="I18" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G18/2&amp; "," &amp;G18/4&amp;  "," &amp;G18&amp;"]"</f>
         <v>[54,27,108]</v>
       </c>
       <c r="J18" s="2">
@@ -1788,11 +1795,11 @@
         <v>0.94810000000000005</v>
       </c>
       <c r="S18" s="7">
-        <f t="shared" si="5"/>
+        <f>(M18+O18+Q18)/3</f>
         <v>34.55266666666666</v>
       </c>
       <c r="T18" s="10">
-        <f t="shared" si="6"/>
+        <f>(N18+P18+R18)/3</f>
         <v>0.95770333333333335</v>
       </c>
     </row>
@@ -1824,7 +1831,7 @@
         <v>13</v>
       </c>
       <c r="I19" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G19/2&amp; "," &amp;G19/4&amp;  "," &amp;G19&amp;"]"</f>
         <v>[6,3,12]</v>
       </c>
       <c r="J19" s="2">
@@ -1836,13 +1843,31 @@
       <c r="L19" s="2">
         <v>1</v>
       </c>
+      <c r="M19" s="7">
+        <v>21.126000000000001</v>
+      </c>
+      <c r="N19" s="13">
+        <v>0.53007000000000004</v>
+      </c>
+      <c r="O19" s="7">
+        <v>26.331</v>
+      </c>
+      <c r="P19" s="10">
+        <v>0.63055000000000005</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>24.882000000000001</v>
+      </c>
+      <c r="R19" s="10">
+        <v>0.52044000000000001</v>
+      </c>
       <c r="S19" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>(M19+O19+Q19)/3</f>
+        <v>24.113</v>
       </c>
       <c r="T19" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>(N19+P19+R19)/3</f>
+        <v>0.56035333333333337</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
@@ -1873,7 +1898,7 @@
         <v>13</v>
       </c>
       <c r="I20" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G20/2&amp; "," &amp;G20/4&amp;  "," &amp;G20&amp;"]"</f>
         <v>[96,48,192]</v>
       </c>
       <c r="J20" s="2">
@@ -1885,13 +1910,31 @@
       <c r="L20" s="2">
         <v>1</v>
       </c>
+      <c r="M20" s="7">
+        <v>30.745000000000001</v>
+      </c>
+      <c r="N20" s="13">
+        <v>0.98060000000000003</v>
+      </c>
+      <c r="O20" s="7">
+        <v>38.472999999999999</v>
+      </c>
+      <c r="P20" s="10">
+        <v>0.98412999999999995</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>37.442</v>
+      </c>
+      <c r="R20" s="10">
+        <v>0.98614999999999997</v>
+      </c>
       <c r="S20" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>(M20+O20+Q20)/3</f>
+        <v>35.553333333333335</v>
       </c>
       <c r="T20" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>(N20+P20+R20)/3</f>
+        <v>0.98362666666666654</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.35">
@@ -1922,7 +1965,7 @@
         <v>13</v>
       </c>
       <c r="I21" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G21/2&amp; "," &amp;G21/4&amp;  "," &amp;G21&amp;"]"</f>
         <v>[96,48,192]</v>
       </c>
       <c r="J21" s="2">
@@ -1934,13 +1977,31 @@
       <c r="L21" s="2">
         <v>1</v>
       </c>
+      <c r="M21" s="7">
+        <v>30.641999999999999</v>
+      </c>
+      <c r="N21" s="13">
+        <v>0.97028999999999999</v>
+      </c>
+      <c r="O21" s="7">
+        <v>37.098999999999997</v>
+      </c>
+      <c r="P21" s="10">
+        <v>0.96301000000000003</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>36.363999999999997</v>
+      </c>
+      <c r="R21" s="10">
+        <v>0.95557999999999998</v>
+      </c>
       <c r="S21" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>(M21+O21+Q21)/3</f>
+        <v>34.701666666666661</v>
       </c>
       <c r="T21" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>(N21+P21+R21)/3</f>
+        <v>0.96295999999999993</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.35">
@@ -1971,7 +2032,7 @@
         <v>13</v>
       </c>
       <c r="I22" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G22/2&amp; "," &amp;G22/4&amp;  "," &amp;G22&amp;"]"</f>
         <v>[96,48,192]</v>
       </c>
       <c r="J22" s="2">
@@ -1983,13 +2044,31 @@
       <c r="L22" s="2">
         <v>1</v>
       </c>
+      <c r="M22" s="7">
+        <v>30.736000000000001</v>
+      </c>
+      <c r="N22" s="13">
+        <v>0.97865999999999997</v>
+      </c>
+      <c r="O22" s="7">
+        <v>38.469000000000001</v>
+      </c>
+      <c r="P22" s="10">
+        <v>0.98348000000000002</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>37.402999999999999</v>
+      </c>
+      <c r="R22" s="10">
+        <v>0.98494999999999999</v>
+      </c>
       <c r="S22" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>(M22+O22+Q22)/3</f>
+        <v>35.536000000000001</v>
       </c>
       <c r="T22" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>(N22+P22+R22)/3</f>
+        <v>0.98236333333333337</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.35">
@@ -2020,7 +2099,7 @@
         <v>13</v>
       </c>
       <c r="I23" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G23/2&amp; "," &amp;G23/4&amp;  "," &amp;G23&amp;"]"</f>
         <v>[96,48,192]</v>
       </c>
       <c r="J23" s="2">
@@ -2032,13 +2111,31 @@
       <c r="L23" s="2">
         <v>1</v>
       </c>
+      <c r="M23" s="7">
+        <v>30.625</v>
+      </c>
+      <c r="N23" s="13">
+        <v>0.96653999999999995</v>
+      </c>
+      <c r="O23" s="7">
+        <v>37.226999999999997</v>
+      </c>
+      <c r="P23" s="10">
+        <v>0.96484000000000003</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>36.35</v>
+      </c>
+      <c r="R23" s="10">
+        <v>0.95452000000000004</v>
+      </c>
       <c r="S23" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>(M23+O23+Q23)/3</f>
+        <v>34.734000000000002</v>
       </c>
       <c r="T23" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>(N23+P23+R23)/3</f>
+        <v>0.96196666666666664</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.35">
@@ -2069,7 +2166,7 @@
         <v>13</v>
       </c>
       <c r="I24" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G24/2&amp; "," &amp;G24/4&amp;  "," &amp;G24&amp;"]"</f>
         <v>[96,48,192]</v>
       </c>
       <c r="J24" s="2">
@@ -2081,13 +2178,31 @@
       <c r="L24" s="2">
         <v>1</v>
       </c>
+      <c r="M24" s="7">
+        <v>30.687000000000001</v>
+      </c>
+      <c r="N24" s="13">
+        <v>0.97135000000000005</v>
+      </c>
+      <c r="O24" s="7">
+        <v>38.4</v>
+      </c>
+      <c r="P24" s="10">
+        <v>0.97996000000000005</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>36.984000000000002</v>
+      </c>
+      <c r="R24" s="10">
+        <v>0.97292999999999996</v>
+      </c>
       <c r="S24" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>(M24+O24+Q24)/3</f>
+        <v>35.356999999999999</v>
       </c>
       <c r="T24" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>(N24+P24+R24)/3</f>
+        <v>0.97474666666666676</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.35">
@@ -2118,7 +2233,7 @@
         <v>13</v>
       </c>
       <c r="I25" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G25/2&amp; "," &amp;G25/4&amp;  "," &amp;G25&amp;"]"</f>
         <v>[96,48,192]</v>
       </c>
       <c r="J25" s="2">
@@ -2130,13 +2245,31 @@
       <c r="L25" s="2">
         <v>1</v>
       </c>
+      <c r="M25" s="7">
+        <v>30.515000000000001</v>
+      </c>
+      <c r="N25" s="13">
+        <v>0.95213999999999999</v>
+      </c>
+      <c r="O25" s="7">
+        <v>38.165999999999997</v>
+      </c>
+      <c r="P25" s="10">
+        <v>0.97552000000000005</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>36.850999999999999</v>
+      </c>
+      <c r="R25" s="10">
+        <v>0.96628000000000003</v>
+      </c>
       <c r="S25" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>(M25+O25+Q25)/3</f>
+        <v>35.17733333333333</v>
       </c>
       <c r="T25" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>(N25+P25+R25)/3</f>
+        <v>0.96464666666666654</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.35">
@@ -2167,7 +2300,7 @@
         <v>13</v>
       </c>
       <c r="I26" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>"[" &amp;G26/2&amp; "," &amp;G26/4&amp;  "," &amp;G26&amp;"]"</f>
         <v>[96,48,192]</v>
       </c>
       <c r="J26" s="2">
@@ -2179,13 +2312,31 @@
       <c r="L26" s="2">
         <v>1</v>
       </c>
+      <c r="M26" s="7">
+        <v>30.678000000000001</v>
+      </c>
+      <c r="N26" s="13">
+        <v>0.96682999999999997</v>
+      </c>
+      <c r="O26" s="7">
+        <v>38.292000000000002</v>
+      </c>
+      <c r="P26" s="10">
+        <v>0.97694000000000003</v>
+      </c>
+      <c r="Q26" s="7">
+        <v>37.198999999999998</v>
+      </c>
+      <c r="R26" s="10">
+        <v>0.97392000000000001</v>
+      </c>
       <c r="S26" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>(M26+O26+Q26)/3</f>
+        <v>35.389666666666663</v>
       </c>
       <c r="T26" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>(N26+P26+R26)/3</f>
+        <v>0.97256333333333334</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.35">
@@ -2193,31 +2344,31 @@
         <v>12</v>
       </c>
       <c r="B27" s="2">
-        <v>2048</v>
+        <v>512</v>
       </c>
       <c r="C27" s="2">
         <v>2</v>
       </c>
       <c r="D27" s="2">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E27" s="2">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F27" s="2">
         <f>((B27-D27)/E27 + 1)^2</f>
-        <v>16129</v>
+        <v>15625</v>
       </c>
       <c r="G27" s="2">
         <f>D27*D27*3</f>
-        <v>3072</v>
+        <v>768</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I27" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>[1536,768,3072]</v>
+        <f>"[" &amp;G27/2&amp; "," &amp;G27/4&amp;  "," &amp;G27&amp;"]"</f>
+        <v>[384,192,768]</v>
       </c>
       <c r="J27" s="2">
         <v>50</v>
@@ -2227,14 +2378,6 @@
       </c>
       <c r="L27" s="2">
         <v>1</v>
-      </c>
-      <c r="S27" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T27" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
@@ -2242,24 +2385,313 @@
         <v>12</v>
       </c>
       <c r="B28" s="2">
-        <v>128</v>
+        <v>1024</v>
       </c>
       <c r="C28" s="2">
         <v>2</v>
+      </c>
+      <c r="D28" s="2">
+        <f>3/128*1024</f>
+        <v>24</v>
+      </c>
+      <c r="E28" s="2">
+        <f>1/128*1024</f>
+        <v>8</v>
+      </c>
+      <c r="F28" s="2">
+        <f>((B28-D28)/E28 + 1)^2</f>
+        <v>15876</v>
+      </c>
+      <c r="G28" s="2">
+        <f>D28*D28*3</f>
+        <v>1728</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" s="2" t="str">
+        <f>"[" &amp;G28/2&amp; "," &amp;G28/4&amp;  "," &amp;G28&amp;"]"</f>
+        <v>[864,432,1728]</v>
+      </c>
+      <c r="J28" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="2">
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2048</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2</v>
+      </c>
+      <c r="D40" s="2">
+        <f>3/128*2048</f>
+        <v>48</v>
+      </c>
+      <c r="E40" s="2">
+        <f>1/128*2048</f>
+        <v>16</v>
+      </c>
+      <c r="F40" s="2">
+        <f t="shared" ref="F40:F45" si="0">((B40-D40)/E40 + 1)^2</f>
+        <v>15876</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" ref="G40:G45" si="1">D40*D40*3</f>
+        <v>6912</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I40" s="2" t="str">
+        <f t="shared" ref="I40:I45" si="2">"[" &amp;G40/2&amp; "," &amp;G40/4&amp;  "," &amp;G40&amp;"]"</f>
+        <v>[3456,1728,6912]</v>
+      </c>
+      <c r="J40" s="2">
+        <v>50</v>
+      </c>
+      <c r="K40" s="2">
+        <v>1</v>
+      </c>
+      <c r="L40" s="2">
+        <v>1</v>
+      </c>
+      <c r="S40" s="7">
+        <f>(M40+O40+Q40)/3</f>
+        <v>0</v>
+      </c>
+      <c r="T40" s="10">
+        <f>(N40+P40+R40)/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="2">
+        <v>2048</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2</v>
+      </c>
+      <c r="D41" s="2">
+        <f>6/128 * 2048</f>
+        <v>96</v>
+      </c>
+      <c r="E41" s="2">
+        <f>1/128*2048</f>
+        <v>16</v>
+      </c>
+      <c r="F41" s="2">
+        <f t="shared" si="0"/>
+        <v>15129</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="1"/>
+        <v>27648</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>[13824,6912,27648]</v>
+      </c>
+      <c r="J41" s="2">
+        <v>50</v>
+      </c>
+      <c r="K41" s="2">
+        <v>1</v>
+      </c>
+      <c r="L41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="2">
+        <v>2048</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2</v>
+      </c>
+      <c r="D42" s="2">
+        <f>8/128*2048</f>
         <v>128</v>
       </c>
-      <c r="C29" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="E42" s="2">
+        <f>1/128*2048</f>
+        <v>16</v>
+      </c>
+      <c r="F42" s="2">
+        <f t="shared" si="0"/>
+        <v>14641</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="1"/>
+        <v>49152</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I42" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>[24576,12288,49152]</v>
+      </c>
+      <c r="J42" s="2">
+        <v>50</v>
+      </c>
+      <c r="K42" s="2">
+        <v>1</v>
+      </c>
+      <c r="L42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="2">
+        <v>2048</v>
+      </c>
+      <c r="C43" s="2">
+        <v>2</v>
+      </c>
+      <c r="D43" s="2">
+        <f>8/128*2048</f>
+        <v>128</v>
+      </c>
+      <c r="E43" s="2">
+        <f>3/128*2048</f>
+        <v>48</v>
+      </c>
+      <c r="F43" s="2">
+        <f t="shared" si="0"/>
+        <v>1681</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="1"/>
+        <v>49152</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I43" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>[24576,12288,49152]</v>
+      </c>
+      <c r="J43" s="2">
+        <v>50</v>
+      </c>
+      <c r="K43" s="2">
+        <v>1</v>
+      </c>
+      <c r="L43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="2">
+        <v>2048</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2</v>
+      </c>
+      <c r="D44" s="2">
+        <f>4/128 * 2048</f>
+        <v>64</v>
+      </c>
+      <c r="E44" s="2">
+        <f>1/128*2048</f>
+        <v>16</v>
+      </c>
+      <c r="F44" s="2">
+        <f t="shared" si="0"/>
+        <v>15625</v>
+      </c>
+      <c r="G44" s="2">
+        <f t="shared" si="1"/>
+        <v>12288</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I44" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>[6144,3072,12288]</v>
+      </c>
+      <c r="J44" s="2">
+        <v>50</v>
+      </c>
+      <c r="K44" s="2">
+        <v>1</v>
+      </c>
+      <c r="L44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2048</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2</v>
+      </c>
+      <c r="D45" s="2">
+        <v>32</v>
+      </c>
+      <c r="E45" s="2">
+        <v>4</v>
+      </c>
+      <c r="F45" s="2">
+        <f t="shared" si="0"/>
+        <v>255025</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="1"/>
+        <v>3072</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>[1536,768,3072]</v>
+      </c>
+      <c r="J45" s="2">
+        <v>50</v>
+      </c>
+      <c r="K45" s="2">
+        <v>1</v>
+      </c>
+      <c r="L45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="J47" s="14"/>
     </row>
     <row r="64" spans="10:10" x14ac:dyDescent="0.35">

</xml_diff>